<commit_message>
add validate on payment_coef
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/companies.xlsx
+++ b/spec/fixtures/files/companies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t xml:space="preserve">company_type</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">payment_coefficient</t>
   </si>
   <si>
     <t xml:space="preserve">phone</t>
@@ -145,6 +148,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -222,31 +226,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="30.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,25 +294,28 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>100010101</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>12312312312</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>17</v>
@@ -321,37 +329,40 @@
       <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>12312312</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>108101123</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>78888733474</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>18</v>
@@ -360,39 +371,42 @@
         <v>19</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>12312322</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>29</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>123213123</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>78474758384</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>18</v>
@@ -401,16 +415,19 @@
         <v>19</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <v>12312313</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="M4" s="0" t="s">
         <v>36</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -418,8 +435,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>